<commit_message>
Add custom keyword for jqueryui datepicker
</commit_message>
<xml_diff>
--- a/Data Files/Accounts.xlsx
+++ b/Data Files/Accounts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A93D14-A96D-BE4C-9120-22424B9D7732}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040F2417-543D-6A43-9CDE-9AA68187817A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valid_accounts" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
     <t>demo@katalon.com</t>
   </si>
   <si>
-    <t>8eml3nBz19rJ6kP8oCYK</t>
-  </si>
-  <si>
     <t>tom@katalon.com</t>
   </si>
   <si>
-    <t>1QpnA1G2cOTSJQLE4U3A</t>
-  </si>
-  <si>
     <t>jerry@katalon.com</t>
   </si>
   <si>
-    <t>K@tAl0n@#1304</t>
-  </si>
-  <si>
     <t>bella@katalon.com</t>
+  </si>
+  <si>
+    <t>sPiHQ&amp;YEa6ST`de+</t>
+  </si>
+  <si>
+    <t>ok{Ikwnm*wzsaEsD</t>
+  </si>
+  <si>
+    <t>gcI#UhR@m(:fsfYU</t>
   </si>
 </sst>
 </file>
@@ -382,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -405,15 +405,15 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -450,15 +450,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -479,7 +479,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -501,23 +501,23 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>